<commit_message>
modified pi hat schematic. Added second temp sensor. Removed Honeywell pressure sensor for two TE sensors
</commit_message>
<xml_diff>
--- a/eagle/projects/raspi_zero_power_sensor_hat/raspi_zero_power_sensor_hat-BOM.xlsx
+++ b/eagle/projects/raspi_zero_power_sensor_hat/raspi_zero_power_sensor_hat-BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="raspi_zero_power_sensor_hat_BOM_1" localSheetId="0">Sheet1!$A$1:$AZ$42</definedName>
+    <definedName name="raspi_zero_power_sensor_hat_BOM_1" localSheetId="0">Sheet1!$A$1:$AW$42</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,10 +33,7 @@
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="raspi_zero_power_sensor_hat-BOM" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/cschwab/Documents/School_Work/RIT_5/Fall_2016/MSD/git_repo/HW/eagle/projects/raspi_zero_power_sensor_hat/raspi_zero_power_sensor_hat-BOM.csv">
-      <textFields count="52">
-        <textField/>
-        <textField/>
-        <textField/>
+      <textFields count="49">
         <textField/>
         <textField/>
         <textField/>
@@ -93,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="316">
   <si>
     <t>Qty</t>
   </si>
@@ -164,12 +161,6 @@
     <t>MAX_CURRENT</t>
   </si>
   <si>
-    <t>MAX_DC_CURRENT</t>
-  </si>
-  <si>
-    <t>MAX_DC_VOLTAGE</t>
-  </si>
-  <si>
     <t>MAX_OUTPUT_CURRENT</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>SHIELDED</t>
   </si>
   <si>
-    <t>SHROUDED</t>
-  </si>
-  <si>
     <t>TEMP_COEFF</t>
   </si>
   <si>
@@ -287,9 +275,6 @@
     <t>C0603</t>
   </si>
   <si>
-    <t>C2, C5, C11, C12, C14, C15, C16, C17, C18</t>
-  </si>
-  <si>
     <t>GRM188R71C104KA01D</t>
   </si>
   <si>
@@ -377,9 +362,6 @@
     <t>LED0603</t>
   </si>
   <si>
-    <t>DS1</t>
-  </si>
-  <si>
     <t>20mA</t>
   </si>
   <si>
@@ -434,45 +416,15 @@
     <t>2,75_HOLE_RASPI</t>
   </si>
   <si>
-    <t>H1, H2, H3, H4</t>
-  </si>
-  <si>
-    <t>JST-PH-2TH-RA</t>
-  </si>
-  <si>
-    <t>JST-PH-2TH-RA_2TH-RA</t>
-  </si>
-  <si>
-    <t>JST-PH-2-THM-RA</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>JST</t>
-  </si>
-  <si>
-    <t>S2B-PH-K-S(LF)(SN)</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>100V</t>
-  </si>
-  <si>
     <t>RIGHT</t>
   </si>
   <si>
-    <t>2.0mm</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>455-1719-ND</t>
-  </si>
-  <si>
     <t>USB_MICROB_RECPT</t>
   </si>
   <si>
@@ -533,27 +485,12 @@
     <t>S1011EC-02-ND</t>
   </si>
   <si>
-    <t>MOL-KK-2-V</t>
-  </si>
-  <si>
-    <t>MOLKK_2PIN2V_2V</t>
-  </si>
-  <si>
-    <t>MOLKK-2-V</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
     <t>Molex</t>
   </si>
   <si>
-    <t>4.0A</t>
-  </si>
-  <si>
-    <t>WM2700-ND</t>
-  </si>
-  <si>
     <t>RECEPTACLE-2x7-2.54MM</t>
   </si>
   <si>
@@ -572,36 +509,6 @@
     <t>S7110-ND</t>
   </si>
   <si>
-    <t>MOL-KK-4-RA</t>
-  </si>
-  <si>
-    <t>MOLKK_4PIN_4RA_RA</t>
-  </si>
-  <si>
-    <t>MOLKK-4-RA</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>WM2713-ND</t>
-  </si>
-  <si>
-    <t>MOL-KK-3P-V</t>
-  </si>
-  <si>
-    <t>MOLKK_3PIN_3V_V</t>
-  </si>
-  <si>
-    <t>MOLKK-3-V</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>WM2701-ND</t>
-  </si>
-  <si>
     <t>J8</t>
   </si>
   <si>
@@ -740,15 +647,9 @@
     <t>RES_0R0_0603</t>
   </si>
   <si>
-    <t>R4, R15, R17, R18, R21</t>
-  </si>
-  <si>
     <t>ERJ-3GEY0R00V</t>
   </si>
   <si>
-    <t>JUMPER</t>
-  </si>
-  <si>
     <t>P0.0GCT-ND</t>
   </si>
   <si>
@@ -818,30 +719,12 @@
     <t>RES_2R0_0603</t>
   </si>
   <si>
-    <t>R10, R11, R23, R24</t>
-  </si>
-  <si>
     <t>ERJ-3EKF2001V</t>
   </si>
   <si>
     <t>P2.00KHCT-ND</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>RES_1R0_0603</t>
-  </si>
-  <si>
-    <t>R12, R13, R14</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1001V</t>
-  </si>
-  <si>
-    <t>P1.00KHCT-ND</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -860,9 +743,6 @@
     <t>RES_4R7_0603</t>
   </si>
   <si>
-    <t>R25</t>
-  </si>
-  <si>
     <t>ERJ-3EKF4701V</t>
   </si>
   <si>
@@ -983,9 +863,6 @@
     <t>SOIC127P130X0600-8N</t>
   </si>
   <si>
-    <t>U6</t>
-  </si>
-  <si>
     <t>I2C</t>
   </si>
   <si>
@@ -995,27 +872,12 @@
     <t>568-10219-1-ND</t>
   </si>
   <si>
-    <t>SSCMNNN015PA2A3</t>
-  </si>
-  <si>
-    <t>SSCMNNN015PA2A3_8SMD</t>
-  </si>
-  <si>
-    <t>SMD254P205X116-8N</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
-    <t>Honeywell</t>
-  </si>
-  <si>
     <t>12b</t>
   </si>
   <si>
-    <t>480-5204-ND</t>
-  </si>
-  <si>
     <t>MAX11613EUA+</t>
   </si>
   <si>
@@ -1067,7 +929,115 @@
     <t>TP10R</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7</t>
+    <t>MOL-SL-2-RA</t>
+  </si>
+  <si>
+    <t>MOLSL_2PIN_SL2RA_RA</t>
+  </si>
+  <si>
+    <t>MOLSL-2-RA</t>
+  </si>
+  <si>
+    <t>WM4900-ND</t>
+  </si>
+  <si>
+    <t>MOL-SL-2-V</t>
+  </si>
+  <si>
+    <t>MOLSL_2PIN_SL2V_V</t>
+  </si>
+  <si>
+    <t>MOLSL-2-V</t>
+  </si>
+  <si>
+    <t>WM4800-ND</t>
+  </si>
+  <si>
+    <t>MOL-SL-4-V</t>
+  </si>
+  <si>
+    <t>MOLSL_4PIN_SL4V_V</t>
+  </si>
+  <si>
+    <t>MOLSL-4-V</t>
+  </si>
+  <si>
+    <t>WM4802-ND</t>
+  </si>
+  <si>
+    <t>MOL-SL-3-V</t>
+  </si>
+  <si>
+    <t>MOLSL_3PIN_SL3V_V</t>
+  </si>
+  <si>
+    <t>MOLSL-3-V</t>
+  </si>
+  <si>
+    <t>WM4801-ND</t>
+  </si>
+  <si>
+    <t>C2, C5, C11, C12, C14, C15, C16, C17, C18, C20</t>
+  </si>
+  <si>
+    <t>DS1, DS7, DS8</t>
+  </si>
+  <si>
+    <t>H4, H5, H6</t>
+  </si>
+  <si>
+    <t>HEADER-1x4-2.54mm</t>
+  </si>
+  <si>
+    <t>HEADER-1X4-254MM_1X4_254MM_TH</t>
+  </si>
+  <si>
+    <t>HEADER-1X4-254MM</t>
+  </si>
+  <si>
+    <t>PRPC004SAAN-RC</t>
+  </si>
+  <si>
+    <t>S1011EC-04-ND</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>R4, R14, R15, R17, R18, R19, R21</t>
+  </si>
+  <si>
+    <t>R5, R10, R11, R12, R13, R20, R22, R30, R31</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP5, TP8, TP9, TP10, TP11, TP12</t>
+  </si>
+  <si>
+    <t>U6, U9</t>
+  </si>
+  <si>
+    <t>MS580305BA01</t>
+  </si>
+  <si>
+    <t>MS5803-05BA_8SMD</t>
+  </si>
+  <si>
+    <t>SMD125130P225X090-8N</t>
+  </si>
+  <si>
+    <t>MS580305BA01-00</t>
+  </si>
+  <si>
+    <t>223-1625-5-ND</t>
   </si>
 </sst>
 </file>
@@ -1388,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ42"/>
+  <dimension ref="A1:AW42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,8 +1369,8 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1419,36 +1389,38 @@
     <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="23.5" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1573,16 +1545,16 @@
         <v>40</v>
       </c>
       <c r="AP1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>314</v>
       </c>
       <c r="AT1" t="s">
         <v>44</v>
@@ -1596,1668 +1568,1674 @@
       <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
+      <c r="U2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="V2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="AM2" t="s">
         <v>54</v>
       </c>
-      <c r="U2" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="AO2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU2" t="s">
         <v>56</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AW2" t="s">
         <v>57</v>
       </c>
-      <c r="AR2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW2" t="s">
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>295</v>
+      </c>
+      <c r="U3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" t="s">
+      <c r="AM3" t="s">
         <v>62</v>
       </c>
-      <c r="D3" t="s">
+      <c r="AO3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
+      <c r="AW3" t="s">
         <v>64</v>
       </c>
-      <c r="U3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="U4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR4" s="1">
+        <v>68</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO4" s="1">
         <v>0.1</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>55</v>
       </c>
       <c r="AU4" t="s">
         <v>69</v>
       </c>
       <c r="AW4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" t="s">
+      <c r="AO5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="AW5" t="s">
         <v>76</v>
       </c>
-      <c r="U5" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR5" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR6" s="1">
+        <v>80</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO6" s="1">
         <v>0.1</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>55</v>
       </c>
       <c r="AU6" t="s">
         <v>81</v>
       </c>
       <c r="AW6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="U7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR7" s="1">
+        <v>85</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO7" s="1">
         <v>0.1</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>55</v>
       </c>
       <c r="AU7" t="s">
         <v>86</v>
       </c>
       <c r="AW7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>296</v>
+      </c>
+      <c r="N8" t="s">
         <v>90</v>
       </c>
-      <c r="AZ7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="O8" t="s">
         <v>91</v>
       </c>
-      <c r="C8" t="s">
+      <c r="U8" t="s">
         <v>92</v>
       </c>
-      <c r="D8" t="s">
+      <c r="V8" t="s">
         <v>93</v>
       </c>
-      <c r="E8" t="s">
+      <c r="AR8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU8" t="s">
         <v>94</v>
       </c>
-      <c r="N8" t="s">
-        <v>95</v>
-      </c>
-      <c r="O8" t="s">
-        <v>96</v>
-      </c>
-      <c r="U8" t="s">
-        <v>97</v>
-      </c>
-      <c r="V8" t="s">
-        <v>98</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N9" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" t="s">
+        <v>98</v>
+      </c>
+      <c r="U9" t="s">
+        <v>92</v>
+      </c>
+      <c r="V9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR9" t="s">
         <v>95</v>
       </c>
-      <c r="O9" t="s">
-        <v>103</v>
-      </c>
-      <c r="U9" t="s">
-        <v>97</v>
-      </c>
-      <c r="V9" t="s">
-        <v>104</v>
+      <c r="AT9" t="s">
+        <v>55</v>
       </c>
       <c r="AU9" t="s">
         <v>100</v>
       </c>
-      <c r="AW9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O10" t="s">
+        <v>91</v>
+      </c>
+      <c r="U10" t="s">
+        <v>92</v>
+      </c>
+      <c r="V10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>106</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-      <c r="N10" t="s">
-        <v>95</v>
-      </c>
-      <c r="O10" t="s">
-        <v>96</v>
-      </c>
-      <c r="U10" t="s">
-        <v>97</v>
-      </c>
-      <c r="V10" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" t="s">
-        <v>112</v>
-      </c>
       <c r="E11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>280</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>281</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>108</v>
+      </c>
+      <c r="M12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S12" t="s">
+        <v>110</v>
       </c>
       <c r="U12" t="s">
-        <v>118</v>
-      </c>
-      <c r="V12" t="s">
-        <v>119</v>
-      </c>
-      <c r="X12" t="s">
-        <v>120</v>
+        <v>132</v>
+      </c>
+      <c r="V12">
+        <v>705530001</v>
+      </c>
+      <c r="W12" t="s">
+        <v>126</v>
       </c>
       <c r="Y12" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>122</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF12">
+        <v>109</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD12">
         <v>2</v>
       </c>
-      <c r="AO12" t="s">
-        <v>124</v>
+      <c r="AR12" t="s">
+        <v>279</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>55</v>
       </c>
       <c r="AU12" t="s">
-        <v>114</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F13">
         <v>5</v>
       </c>
       <c r="U13" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="V13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>132</v>
+        <v>116</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>55</v>
       </c>
       <c r="AU13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="M14" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="U14" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="V14" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="W14" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF14">
+        <v>126</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD14">
         <v>2</v>
       </c>
-      <c r="AL14">
+      <c r="AJ14">
         <v>1</v>
       </c>
+      <c r="AR14" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>55</v>
+      </c>
       <c r="AU14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>283</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>285</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M15" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="S15" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="U15" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="V15">
-        <v>22112022</v>
+        <v>705430001</v>
       </c>
       <c r="W15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF15">
+        <v>126</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD15">
         <v>2</v>
       </c>
+      <c r="AR15" t="s">
+        <v>283</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>55</v>
+      </c>
       <c r="AU15" t="s">
-        <v>146</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="M16" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="U16" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="V16" t="s">
-        <v>157</v>
+        <v>301</v>
       </c>
       <c r="W16" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF16">
-        <v>14</v>
-      </c>
-      <c r="AL16">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD16">
+        <v>4</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>298</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>55</v>
       </c>
       <c r="AU16" t="s">
-        <v>153</v>
-      </c>
-      <c r="AW16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>270</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>271</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>272</v>
       </c>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="M17" t="s">
-        <v>138</v>
-      </c>
-      <c r="S17" t="s">
+        <v>123</v>
+      </c>
+      <c r="U17" t="s">
         <v>124</v>
       </c>
-      <c r="U17" t="s">
-        <v>150</v>
-      </c>
-      <c r="V17">
-        <v>22122044</v>
+      <c r="V17" t="s">
+        <v>273</v>
       </c>
       <c r="W17" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF17">
-        <v>4</v>
+        <v>126</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>274</v>
+      </c>
+      <c r="AD17">
+        <v>5</v>
+      </c>
+      <c r="AJ17">
+        <v>1</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>270</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>55</v>
       </c>
       <c r="AU17" t="s">
-        <v>159</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>167</v>
+        <v>303</v>
       </c>
       <c r="M18" t="s">
+        <v>123</v>
+      </c>
+      <c r="U18" t="s">
+        <v>124</v>
+      </c>
+      <c r="V18" t="s">
+        <v>137</v>
+      </c>
+      <c r="W18" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD18">
+        <v>14</v>
+      </c>
+      <c r="AJ18">
+        <v>2</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>133</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU18" t="s">
         <v>138</v>
       </c>
-      <c r="S18" t="s">
-        <v>124</v>
-      </c>
-      <c r="U18" t="s">
-        <v>150</v>
-      </c>
-      <c r="V18">
-        <v>22112032</v>
-      </c>
-      <c r="W18" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF18">
-        <v>3</v>
-      </c>
-      <c r="AU18" t="s">
-        <v>164</v>
-      </c>
-      <c r="AW18" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="C19" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="D19" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
       <c r="E19" t="s">
-        <v>169</v>
+        <v>304</v>
       </c>
       <c r="M19" t="s">
-        <v>138</v>
+        <v>123</v>
+      </c>
+      <c r="S19" t="s">
+        <v>110</v>
       </c>
       <c r="U19" t="s">
-        <v>139</v>
-      </c>
-      <c r="V19" t="s">
-        <v>318</v>
+        <v>132</v>
+      </c>
+      <c r="V19">
+        <v>705430003</v>
       </c>
       <c r="W19" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>319</v>
-      </c>
-      <c r="AF19">
-        <v>5</v>
-      </c>
-      <c r="AL19">
-        <v>1</v>
+        <v>126</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD19">
+        <v>4</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>287</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>55</v>
       </c>
       <c r="AU19" t="s">
-        <v>315</v>
-      </c>
-      <c r="AW19" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX19" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>293</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
-      </c>
-      <c r="H20" t="s">
-        <v>174</v>
-      </c>
-      <c r="I20" t="s">
-        <v>175</v>
-      </c>
-      <c r="J20" t="s">
-        <v>176</v>
+        <v>305</v>
+      </c>
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+      <c r="S20" t="s">
+        <v>110</v>
       </c>
       <c r="U20" t="s">
-        <v>177</v>
-      </c>
-      <c r="V20" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>179</v>
-      </c>
-      <c r="AR20" s="1">
+        <v>132</v>
+      </c>
+      <c r="V20">
+        <v>705430002</v>
+      </c>
+      <c r="W20" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD20">
+        <v>3</v>
+      </c>
+      <c r="AO20" s="1"/>
+      <c r="AR20" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" t="s">
+        <v>145</v>
+      </c>
+      <c r="J21" t="s">
+        <v>146</v>
+      </c>
+      <c r="U21" t="s">
+        <v>147</v>
+      </c>
+      <c r="V21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO21" s="1">
         <v>0.2</v>
       </c>
-      <c r="AT20" t="s">
-        <v>180</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>170</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="AQ21" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>182</v>
-      </c>
-      <c r="C21" t="s">
-        <v>183</v>
-      </c>
-      <c r="D21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E21" t="s">
-        <v>185</v>
-      </c>
-      <c r="G21" t="s">
-        <v>175</v>
-      </c>
-      <c r="L21" t="s">
-        <v>186</v>
-      </c>
-      <c r="U21" t="s">
-        <v>187</v>
-      </c>
-      <c r="V21" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>190</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>182</v>
-      </c>
-      <c r="AV21" t="s">
-        <v>191</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX21" t="s">
-        <v>192</v>
-      </c>
-      <c r="AY21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>0.05</v>
+      <c r="B22" t="s">
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>155</v>
+      </c>
+      <c r="G22" t="s">
+        <v>145</v>
+      </c>
+      <c r="L22" t="s">
+        <v>156</v>
       </c>
       <c r="U22" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="V22" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ22">
-        <v>4</v>
-      </c>
-      <c r="AR22" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AU22">
-        <v>0.05</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO22" s="2"/>
+      <c r="AR22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>162</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>201</v>
+      <c r="B23">
+        <v>0.05</v>
       </c>
       <c r="C23" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="E23" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="U23" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="V23" t="s">
-        <v>206</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>207</v>
+        <v>168</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN23">
+        <v>4</v>
+      </c>
+      <c r="AO23" s="1">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AR23" s="1">
-        <v>0.01</v>
+        <v>0.05</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>55</v>
       </c>
       <c r="AU23" t="s">
-        <v>201</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX23" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
+        <v>174</v>
+      </c>
+      <c r="U24" t="s">
+        <v>175</v>
+      </c>
+      <c r="V24" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+      <c r="U25" t="s">
+        <v>175</v>
+      </c>
+      <c r="V25" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" t="s">
+        <v>306</v>
+      </c>
+      <c r="U26" t="s">
+        <v>175</v>
+      </c>
+      <c r="V26" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO26" s="1"/>
+      <c r="AR26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" t="s">
+        <v>307</v>
+      </c>
+      <c r="U27" t="s">
+        <v>175</v>
+      </c>
+      <c r="V27" t="s">
         <v>209</v>
       </c>
-      <c r="C24" t="s">
+      <c r="AE27" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO27" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU27" t="s">
         <v>210</v>
       </c>
-      <c r="D24" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" t="s">
-        <v>211</v>
-      </c>
-      <c r="U24" t="s">
-        <v>205</v>
-      </c>
-      <c r="V24" t="s">
-        <v>212</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR24" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AU24" t="s">
-        <v>209</v>
-      </c>
-      <c r="AW24" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>214</v>
-      </c>
-      <c r="D25" t="s">
-        <v>203</v>
-      </c>
-      <c r="E25" t="s">
-        <v>215</v>
-      </c>
-      <c r="U25" t="s">
-        <v>205</v>
-      </c>
-      <c r="V25" t="s">
-        <v>216</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>217</v>
-      </c>
-      <c r="AU25">
-        <v>0</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" t="s">
-        <v>220</v>
-      </c>
-      <c r="D26" t="s">
-        <v>203</v>
-      </c>
-      <c r="E26" t="s">
-        <v>221</v>
-      </c>
-      <c r="U26" t="s">
-        <v>205</v>
-      </c>
-      <c r="V26" t="s">
-        <v>222</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR26" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AU26" t="s">
-        <v>219</v>
-      </c>
-      <c r="AW26" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX26" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>224</v>
-      </c>
-      <c r="C27" t="s">
-        <v>225</v>
-      </c>
-      <c r="D27" t="s">
-        <v>203</v>
-      </c>
-      <c r="E27" t="s">
-        <v>226</v>
-      </c>
-      <c r="U27" t="s">
-        <v>205</v>
-      </c>
-      <c r="V27" t="s">
-        <v>227</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR27" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AU27" t="s">
-        <v>224</v>
-      </c>
-      <c r="AW27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX27" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="C28" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="D28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" t="s">
+        <v>189</v>
+      </c>
+      <c r="U28" t="s">
+        <v>175</v>
+      </c>
+      <c r="V28" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO28" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" t="s">
+        <v>194</v>
+      </c>
+      <c r="U29" t="s">
+        <v>175</v>
+      </c>
+      <c r="V29" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO29" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR29" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" t="s">
+        <v>199</v>
+      </c>
+      <c r="U30" t="s">
+        <v>175</v>
+      </c>
+      <c r="V30" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO30" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AR30" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>49.9</v>
+      </c>
+      <c r="C31" t="s">
         <v>203</v>
       </c>
-      <c r="E28" t="s">
-        <v>231</v>
-      </c>
-      <c r="U28" t="s">
+      <c r="D31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" t="s">
+        <v>204</v>
+      </c>
+      <c r="U31" t="s">
+        <v>175</v>
+      </c>
+      <c r="V31" t="s">
         <v>205</v>
       </c>
-      <c r="V28" t="s">
-        <v>232</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>233</v>
-      </c>
-      <c r="AR28" s="1">
+      <c r="AE31" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO31" s="1">
         <v>0.01</v>
       </c>
-      <c r="AU28" t="s">
-        <v>229</v>
-      </c>
-      <c r="AW28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29">
+      <c r="AR31" s="1">
         <v>49.9</v>
       </c>
-      <c r="C29" t="s">
-        <v>235</v>
-      </c>
-      <c r="D29" t="s">
-        <v>203</v>
-      </c>
-      <c r="E29" t="s">
-        <v>236</v>
-      </c>
-      <c r="U29" t="s">
-        <v>205</v>
-      </c>
-      <c r="V29" t="s">
-        <v>237</v>
-      </c>
-      <c r="AG29" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR29" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AU29">
-        <v>49.9</v>
-      </c>
-      <c r="AW29" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>239</v>
-      </c>
-      <c r="C30" t="s">
-        <v>240</v>
-      </c>
-      <c r="D30" t="s">
-        <v>203</v>
-      </c>
-      <c r="E30" t="s">
-        <v>241</v>
-      </c>
-      <c r="U30" t="s">
-        <v>205</v>
-      </c>
-      <c r="V30" t="s">
-        <v>242</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR30" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="AU30" t="s">
-        <v>239</v>
-      </c>
-      <c r="AW30" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX30" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>244</v>
-      </c>
-      <c r="C31" t="s">
-        <v>245</v>
-      </c>
-      <c r="D31" t="s">
-        <v>203</v>
-      </c>
-      <c r="E31" t="s">
-        <v>246</v>
-      </c>
-      <c r="U31" t="s">
-        <v>205</v>
-      </c>
-      <c r="V31" t="s">
-        <v>247</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR31" s="1">
-        <v>0.01</v>
+      <c r="AT31" t="s">
+        <v>55</v>
       </c>
       <c r="AU31" t="s">
-        <v>244</v>
-      </c>
-      <c r="AW31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX31" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="C32" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="D32" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="E32" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="U32" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="V32" t="s">
-        <v>251</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR32" s="1">
+        <v>213</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO32" s="1">
         <v>0.01</v>
       </c>
+      <c r="AR32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>55</v>
+      </c>
       <c r="AU32" t="s">
-        <v>249</v>
-      </c>
-      <c r="AW32" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX32" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="C33" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="D33" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="E33" t="s">
-        <v>255</v>
+        <v>308</v>
       </c>
       <c r="U33" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="V33" t="s">
-        <v>256</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR33" s="1">
+        <v>217</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO33" s="1">
         <v>0.01</v>
       </c>
+      <c r="AR33" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>55</v>
+      </c>
       <c r="AU33" t="s">
-        <v>253</v>
-      </c>
-      <c r="AW33" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX33" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>322</v>
+        <v>277</v>
       </c>
       <c r="D34" t="s">
-        <v>323</v>
+        <v>278</v>
       </c>
       <c r="E34" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
-        <v>259</v>
+        <v>220</v>
       </c>
       <c r="D35" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="E35" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="P35" t="s">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="T35" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="U35" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="V35" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>266</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>267</v>
+        <v>226</v>
+      </c>
+      <c r="X35" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>228</v>
+      </c>
+      <c r="AR35" t="s">
+        <v>219</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>55</v>
       </c>
       <c r="AU35" t="s">
-        <v>258</v>
-      </c>
-      <c r="AW35" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX35" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="E36" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="U36" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="V36" t="s">
-        <v>269</v>
+        <v>230</v>
+      </c>
+      <c r="AR36" t="s">
+        <v>230</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>234</v>
       </c>
       <c r="AU36" t="s">
-        <v>269</v>
-      </c>
-      <c r="AW36" t="s">
-        <v>273</v>
-      </c>
-      <c r="AX36" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="C37" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="D37" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="E37" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="U37" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="V37" t="s">
-        <v>274</v>
+        <v>235</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>55</v>
       </c>
       <c r="AU37" t="s">
-        <v>274</v>
-      </c>
-      <c r="AW37" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C38" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="D38" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="E38" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
       <c r="U38" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="V38" t="s">
-        <v>279</v>
+        <v>240</v>
+      </c>
+      <c r="AR38" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>55</v>
       </c>
       <c r="AU38" t="s">
-        <v>278</v>
-      </c>
-      <c r="AW38" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX38" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s">
-        <v>285</v>
+        <v>246</v>
       </c>
       <c r="D39" t="s">
-        <v>286</v>
+        <v>247</v>
       </c>
       <c r="E39" t="s">
-        <v>287</v>
+        <v>248</v>
       </c>
       <c r="Q39" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="U39" t="s">
-        <v>289</v>
+        <v>250</v>
       </c>
       <c r="V39" t="s">
-        <v>284</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>290</v>
-      </c>
-      <c r="AI39" t="s">
-        <v>291</v>
+        <v>245</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>252</v>
+      </c>
+      <c r="AR39" t="s">
+        <v>245</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>55</v>
       </c>
       <c r="AU39" t="s">
-        <v>284</v>
-      </c>
-      <c r="AW39" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX39" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="C40" t="s">
-        <v>294</v>
+        <v>255</v>
       </c>
       <c r="D40" t="s">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="E40" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="Q40" t="s">
-        <v>297</v>
+        <v>257</v>
       </c>
       <c r="U40" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="V40" t="s">
-        <v>293</v>
-      </c>
-      <c r="AK40" t="s">
-        <v>298</v>
+        <v>254</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>258</v>
+      </c>
+      <c r="AR40" t="s">
+        <v>254</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>55</v>
       </c>
       <c r="AU40" t="s">
-        <v>293</v>
-      </c>
-      <c r="AW40" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX40" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="C41" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="D41" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="E41" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="Q41" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="U41" t="s">
-        <v>304</v>
+        <v>250</v>
       </c>
       <c r="V41" t="s">
-        <v>300</v>
-      </c>
-      <c r="AC41" t="s">
-        <v>305</v>
-      </c>
-      <c r="AI41" t="s">
-        <v>291</v>
+        <v>314</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>252</v>
+      </c>
+      <c r="AR41" t="s">
+        <v>311</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>55</v>
       </c>
       <c r="AU41" t="s">
-        <v>300</v>
-      </c>
-      <c r="AW41" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX41" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="C42" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="D42" t="s">
-        <v>308</v>
+        <v>263</v>
       </c>
       <c r="E42" t="s">
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="R42" t="s">
-        <v>310</v>
+        <v>265</v>
       </c>
       <c r="U42" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="V42" t="s">
-        <v>307</v>
+        <v>262</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>261</v>
       </c>
       <c r="AK42" t="s">
-        <v>305</v>
-      </c>
-      <c r="AM42" t="s">
-        <v>312</v>
+        <v>267</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>262</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>55</v>
       </c>
       <c r="AU42" t="s">
-        <v>307</v>
-      </c>
-      <c r="AW42" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX42" t="s">
-        <v>313</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>